<commit_message>
working container string parsing on distributions parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-distribution.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-distribution.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
@@ -160,6 +160,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="N3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>List of the tanks/cups/trays fish were taken from for distributions. 
+Format: 
+Tanks: raw number: 1, 4, 6-9
+Trays: single dot: 1.1, 2.3, 4.5-6.7
+Cups: double dot: 1.1.1, 2.2.2, 3.3.3-4.4.4
+Multiple: 7-9, 1.3, 2.3.4-5.6.7
+Separate items with commas, can use hypens for sequential containers. Use spaces as needed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="P3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -169,46 +201,46 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
+          <t>Optional, in C</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional, in C</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
           <t>Optional</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Optional, in C</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Optional, in C</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Optional</t>
+    <comment ref="T3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Optional, units can be (cm) or (mm)</t>
         </r>
       </text>
     </comment>
@@ -221,24 +253,11 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Optional, units can be (cm) or (mm)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
           <t>Optional, units can be (kg) or (g).</t>
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="0" shapeId="0">
+    <comment ref="W3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -474,7 +493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Year</t>
   </si>
@@ -558,13 +577,16 @@
   </si>
   <si>
     <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>Container</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,6 +599,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -898,26 +926,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:X3"/>
+  <dimension ref="A3:W3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3:V3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="28.28515625" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.140625" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -958,36 +986,33 @@
         <v>16</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1002,13 +1027,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="13" max="14" width="14.7109375" customWidth="1"/>
     <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
add exclude column to distributions parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-distribution.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-distribution.xlsx
@@ -186,13 +186,26 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>cups and drawers to be excluded from containers listed. Eg: 3.4 to exclude drawer, 3.4.5 to exclude cup.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
           <t>Optional</t>
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0">
+    <comment ref="Q3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -205,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0">
+    <comment ref="R3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0">
+    <comment ref="S3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -231,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0">
+    <comment ref="U3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -244,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0">
+    <comment ref="V3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -257,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W3" authorId="0" shapeId="0">
+    <comment ref="X3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -493,7 +506,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Year</t>
   </si>
@@ -580,6 +593,9 @@
   </si>
   <si>
     <t>Container</t>
+  </si>
+  <si>
+    <t>Exclude</t>
   </si>
 </sst>
 </file>
@@ -926,26 +942,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:W3"/>
+  <dimension ref="A3:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="28.28515625" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="14" max="14" width="27.140625" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="27.140625" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -989,30 +1005,33 @@
         <v>28</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add in lifestage columns, #855
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-distribution.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-distribution.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
@@ -244,6 +244,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="T3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use full name
+Eg. Fry/Parr/Smolt</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="U3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -433,6 +447,20 @@
             <charset val="1"/>
           </rPr>
           <t>Optional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use full name
+Eg. Fry/Parr/Smolt</t>
         </r>
       </text>
     </comment>
@@ -944,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:X4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add mark to distributions, fix sites.clean()
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-distribution.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-distribution.xlsx
@@ -169,6 +169,20 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">Optional, If filled, must match mark in database e.g. Adipose Clip
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>List of the tanks/cups/trays fish were taken from for distributions. 
 Format: 
 Tanks: raw number: 1, 4, 6-9
@@ -179,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0">
+    <comment ref="P3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -192,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0">
+    <comment ref="Q3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -205,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0">
+    <comment ref="R3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0">
+    <comment ref="S3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -231,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0" shapeId="0">
+    <comment ref="T3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -244,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0">
+    <comment ref="U3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -258,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0">
+    <comment ref="V3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0">
+    <comment ref="W3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="0" shapeId="0">
+    <comment ref="Y3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -459,12 +473,26 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">Optional, If filled, must match mark in database e.g. Adipose Clip
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Use full name
 Eg. Fry/Parr/Smolt</t>
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0">
+    <comment ref="U3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -477,7 +505,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0">
+    <comment ref="V3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -490,7 +518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0">
+    <comment ref="W3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -503,7 +531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W3" authorId="0" shapeId="0">
+    <comment ref="X3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -516,7 +544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="0" shapeId="0">
+    <comment ref="Y3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -534,7 +562,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Year</t>
   </si>
@@ -624,6 +652,9 @@
   </si>
   <si>
     <t>Exclude</t>
+  </si>
+  <si>
+    <t>Mark</t>
   </si>
 </sst>
 </file>
@@ -970,26 +1001,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:X3"/>
+  <dimension ref="A3:Y3"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="28.28515625" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="14" max="15" width="27.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="27.140625" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1030,36 +1061,39 @@
         <v>16</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1072,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:X4"/>
+  <dimension ref="A3:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,14 +1120,15 @@
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" customWidth="1"/>
+    <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1149,25 +1184,28 @@
         <v>21</v>
       </c>
       <c r="S3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
     </row>
   </sheetData>

</xml_diff>